<commit_message>
basic documentation with the simple table within a spreadsheet
</commit_message>
<xml_diff>
--- a/src/test/resources/examples/basic_examples.xlsx
+++ b/src/test/resources/examples/basic_examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Developer/vortexa/refinery/src/test/resources/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F9433E-1670-2D43-B3D8-8B11311FE48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C9D2A6-06A7-D040-BB96-98F4441DFE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
+    <workbookView xWindow="5900" yWindow="4160" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
   </bookViews>
   <sheets>
     <sheet name="simple spreadsheet" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="A1:F5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,6 +584,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add multiple tables test example
</commit_message>
<xml_diff>
--- a/src/test/resources/examples/basic_examples.xlsx
+++ b/src/test/resources/examples/basic_examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Developer/vortexa/refinery/src/test/resources/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C9D2A6-06A7-D040-BB96-98F4441DFE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF837AC3-77FC-234F-B78F-D1F19AB78C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="4160" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
+    <workbookView xWindow="5900" yWindow="4160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
   </bookViews>
   <sheets>
     <sheet name="simple spreadsheet" sheetId="1" r:id="rId1"/>
@@ -77,12 +77,6 @@
     <t>guest team</t>
   </si>
   <si>
-    <t>home_score</t>
-  </si>
-  <si>
-    <t>guest_score</t>
-  </si>
-  <si>
     <t>Group A</t>
   </si>
   <si>
@@ -99,6 +93,12 @@
   </si>
   <si>
     <t>AC Milan</t>
+  </si>
+  <si>
+    <t>home score</t>
+  </si>
+  <si>
+    <t>guest score</t>
   </si>
 </sst>
 </file>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC8572E-3DF2-AD4E-BF7C-D66146F56C14}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,10 +710,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
@@ -845,6 +845,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -852,7 +853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8423F4D-2F30-2E44-BF48-B1C34CC84E3C}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -860,7 +861,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -926,7 +927,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -942,7 +943,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -953,7 +954,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -964,7 +965,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -975,7 +976,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>3</v>

</xml_diff>

<commit_message>
add multiple tables with anchors test example, fix anchor matching
</commit_message>
<xml_diff>
--- a/src/test/resources/examples/basic_examples.xlsx
+++ b/src/test/resources/examples/basic_examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Developer/vortexa/refinery/src/test/resources/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF837AC3-77FC-234F-B78F-D1F19AB78C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE340875-A030-484B-9FAC-0C86CDC16379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="4160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
+    <workbookView xWindow="5900" yWindow="4160" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
   </bookViews>
   <sheets>
     <sheet name="simple spreadsheet" sheetId="1" r:id="rId1"/>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC8572E-3DF2-AD4E-BF7C-D66146F56C14}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -853,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8423F4D-2F30-2E44-BF48-B1C34CC84E3C}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add more examples, remove Test prefix from the examples (Example suffix will be enough)
</commit_message>
<xml_diff>
--- a/src/test/resources/examples/basic_examples.xlsx
+++ b/src/test/resources/examples/basic_examples.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Developer/vortexa/refinery/src/test/resources/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C145F50-206E-FD42-AAF6-B05D74828A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42DDA33-E189-1B48-8114-FBED18868526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="2640" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
+    <workbookView xWindow="5880" yWindow="3380" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
   </bookViews>
   <sheets>
     <sheet name="simple spreadsheet" sheetId="1" r:id="rId1"/>
     <sheet name="multiple tables" sheetId="2" r:id="rId2"/>
     <sheet name="multiple tables with anchors" sheetId="3" r:id="rId3"/>
+    <sheet name="table with dividers" sheetId="4" r:id="rId4"/>
+    <sheet name="data with merged cells" sheetId="5" r:id="rId5"/>
+    <sheet name="merged cells header" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'simple spreadsheet'!$A$1:$E$1</definedName>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="21">
   <si>
     <t>team</t>
   </si>
@@ -99,6 +102,9 @@
   </si>
   <si>
     <t>guest score</t>
+  </si>
+  <si>
+    <t>score</t>
   </si>
 </sst>
 </file>
@@ -150,13 +156,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,7 +608,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A9" sqref="A9:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -853,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8423F4D-2F30-2E44-BF48-B1C34CC84E3C}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -989,4 +1004,344 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4610A78-26A3-F04B-8FA6-61A96ABD5789}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78A6320-FAC2-AD4C-A448-C3AF2EA1E01D}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B558C4-57BE-6448-8AAC-7240F0870BFB}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3">
+        <v>44454</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>44454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>44467</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>44467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3">
+        <v>44488</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44488</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
transformation example, fix exceptions handling found during the regression
</commit_message>
<xml_diff>
--- a/src/test/resources/examples/basic_examples.xlsx
+++ b/src/test/resources/examples/basic_examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Developer/vortexa/refinery/src/test/resources/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42DDA33-E189-1B48-8114-FBED18868526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D883C8B-01F0-5640-9B19-8D7F293FE7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="3380" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
+    <workbookView xWindow="440" yWindow="540" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
   </bookViews>
   <sheets>
     <sheet name="simple spreadsheet" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="table with dividers" sheetId="4" r:id="rId4"/>
     <sheet name="data with merged cells" sheetId="5" r:id="rId5"/>
     <sheet name="merged cells header" sheetId="6" r:id="rId6"/>
+    <sheet name="broken stats" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'simple spreadsheet'!$A$1:$E$1</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="21">
   <si>
     <t>team</t>
   </si>
@@ -136,12 +137,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -172,6 +185,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,7 +505,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,7 +624,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:E15"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1011,7 +1027,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C11" sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1212,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B558C4-57BE-6448-8AAC-7240F0870BFB}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1344,4 +1360,223 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD202F1F-E398-004F-9173-09CCA4229C40}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2">
+        <v>44502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2">
+        <v>44502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>-3</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="2">
+        <v>44502</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>-5</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>44502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2">
+        <v>44504</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>-3</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>44504</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2">
+        <v>44504</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>44504</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix locating the divider by checking the table's min column index and max column index
</commit_message>
<xml_diff>
--- a/src/test/resources/examples/basic_examples.xlsx
+++ b/src/test/resources/examples/basic_examples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Developer/vortexa/refinery/src/test/resources/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D883C8B-01F0-5640-9B19-8D7F293FE7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC50ECB-D059-D043-A625-68550ACAA10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="540" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
+    <workbookView xWindow="440" yWindow="540" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
   </bookViews>
   <sheets>
     <sheet name="simple spreadsheet" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="data with merged cells" sheetId="5" r:id="rId5"/>
     <sheet name="merged cells header" sheetId="6" r:id="rId6"/>
     <sheet name="broken stats" sheetId="7" r:id="rId7"/>
+    <sheet name="table with merged dividers" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'simple spreadsheet'!$A$1:$E$1</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="22">
   <si>
     <t>team</t>
   </si>
@@ -106,6 +107,9 @@
   </si>
   <si>
     <t>score</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -169,25 +173,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4610A78-26A3-F04B-8FA6-61A96ABD5789}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="A1:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1044,11 +1051,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1095,11 +1102,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1182,7 +1189,7 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="10">
         <v>3</v>
       </c>
       <c r="C2">
@@ -1193,7 +1200,7 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="10"/>
       <c r="C3">
         <v>6</v>
       </c>
@@ -1202,7 +1209,7 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="10"/>
       <c r="C4">
         <v>4</v>
       </c>
@@ -1211,7 +1218,7 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="10"/>
       <c r="C5">
         <v>0</v>
       </c>
@@ -1244,10 +1251,10 @@
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1366,7 +1373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD202F1F-E398-004F-9173-09CCA4229C40}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1450,7 +1457,7 @@
       <c r="D5">
         <v>-3</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="2">
         <v>44502</v>
       </c>
@@ -1550,8 +1557,8 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10">
+      <c r="D13" s="6"/>
+      <c r="E13" s="7">
         <v>4</v>
       </c>
       <c r="F13" s="2">
@@ -1568,7 +1575,7 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="6"/>
       <c r="E14">
         <v>1</v>
       </c>
@@ -1579,4 +1586,154 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA12AB0C-2095-0640-82DD-B55C02D33507}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="A2:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add allowedDividers feature (#47)
</commit_message>
<xml_diff>
--- a/src/test/resources/examples/basic_examples.xlsx
+++ b/src/test/resources/examples/basic_examples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\stefbg\projects\refinery\src\test\resources\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/code/refinery/src/test/resources/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0938FEB9-DBCE-4371-8CB1-2ABFFD523ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B837BB-8D08-3D4A-9110-E171069A78EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="7" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="8" xr2:uid="{49CDDE8F-BA7F-BF4B-BD65-A3497930864D}"/>
   </bookViews>
   <sheets>
     <sheet name="simple spreadsheet" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="merged cells header" sheetId="6" r:id="rId6"/>
     <sheet name="broken stats" sheetId="7" r:id="rId7"/>
     <sheet name="table with merged dividers" sheetId="8" r:id="rId8"/>
+    <sheet name="table with constrained dividers" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'simple spreadsheet'!$A$1:$E$1</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="25">
   <si>
     <t>team</t>
   </si>
@@ -113,6 +114,12 @@
   </si>
   <si>
     <t>ignored</t>
+  </si>
+  <si>
+    <t>Group that is to be ignored as a divider</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
   </si>
 </sst>
 </file>
@@ -176,15 +183,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -518,12 +523,12 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -563,7 +568,7 @@
         <v>44502</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -583,7 +588,7 @@
         <v>44502</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -603,7 +608,7 @@
         <v>44502</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -637,13 +642,13 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -683,7 +688,7 @@
         <v>44502</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -703,7 +708,7 @@
         <v>44502</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -723,7 +728,7 @@
         <v>44502</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -743,7 +748,7 @@
         <v>44502</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -760,14 +765,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>6</v>
       </c>
       <c r="D10">
@@ -777,7 +782,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -794,7 +799,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -811,7 +816,7 @@
         <v>44467</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -828,7 +833,7 @@
         <v>44467</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -845,7 +850,7 @@
         <v>44488</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -862,7 +867,7 @@
         <v>44488</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -873,7 +878,7 @@
         <v>44503</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -898,14 +903,14 @@
       <selection activeCell="C6" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -918,7 +923,7 @@
       <c r="D2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -930,7 +935,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -942,7 +947,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -954,7 +959,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -966,12 +971,12 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -982,7 +987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -993,7 +998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1004,7 +1009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1015,7 +1020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1037,12 +1042,12 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+      <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1053,14 +1058,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1071,7 +1076,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1082,7 +1087,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1093,7 +1098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1104,14 +1109,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1122,7 +1127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1133,7 +1138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1144,7 +1149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1172,12 +1177,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1188,40 +1193,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>3</v>
       </c>
       <c r="C2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="8"/>
       <c r="C3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="8"/>
       <c r="C4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="8"/>
       <c r="C5">
         <v>0</v>
       </c>
@@ -1242,34 +1247,34 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="11"/>
+      <c r="D1" s="9"/>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2">
         <v>6</v>
       </c>
       <c r="D2">
@@ -1279,7 +1284,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1296,7 +1301,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1313,7 +1318,7 @@
         <v>44467</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1330,7 +1335,7 @@
         <v>44467</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1347,7 +1352,7 @@
         <v>44488</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1380,14 +1385,14 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1407,7 +1412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1427,7 +1432,7 @@
         <v>44502</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1447,7 +1452,7 @@
         <v>44502</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1460,12 +1465,12 @@
       <c r="D5">
         <v>-3</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="2">
         <v>44502</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1485,12 +1490,12 @@
         <v>44502</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1510,7 +1515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1530,7 +1535,7 @@
         <v>44504</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1550,7 +1555,7 @@
         <v>44504</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1560,15 +1565,15 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7">
+      <c r="D13" s="5"/>
+      <c r="E13">
         <v>4</v>
       </c>
       <c r="F13" s="2">
         <v>44504</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1578,7 +1583,7 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="5"/>
       <c r="E14">
         <v>1</v>
       </c>
@@ -1595,18 +1600,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA12AB0C-2095-0640-82DD-B55C02D33507}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1620,19 +1625,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1643,7 +1648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1654,7 +1659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1665,7 +1670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1676,22 +1681,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="D8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1702,7 +1707,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1713,7 +1718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1724,7 +1729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1742,4 +1747,152 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33749CCB-F98A-974A-8443-287AFFE2BA37}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>